<commit_message>
use gralde to update the resource file
</commit_message>
<xml_diff>
--- a/datasource/src/main/resources/arrangement.xlsx
+++ b/datasource/src/main/resources/arrangement.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bkang016/work-station/git-repository/BuildingGuide/app/src/main/res/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bkang016/work-station/git-repository/BuildingGuide/datasource/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -39,25 +39,25 @@
     <t>group_name</t>
   </si>
   <si>
+    <t>中国华电集团公司</t>
+  </si>
+  <si>
+    <t>上海华滨投资有限公司</t>
+  </si>
+  <si>
+    <t>华鑫国际信托有限公司</t>
+  </si>
+  <si>
+    <t>华远星海运有限公司</t>
+  </si>
+  <si>
+    <t>华电重工股份有限公司上海分公司</t>
+  </si>
+  <si>
+    <t>上海公司</t>
+  </si>
+  <si>
     <t>上海通华燃气轮机服务有限公司</t>
-  </si>
-  <si>
-    <t>中国华电集团公司</t>
-  </si>
-  <si>
-    <t>上海华滨投资有限公司</t>
-  </si>
-  <si>
-    <t>华鑫国际信托有限公司</t>
-  </si>
-  <si>
-    <t>华远星海运有限公司</t>
-  </si>
-  <si>
-    <t>华电重工股份有限公司上海分公司</t>
-  </si>
-  <si>
-    <t>上海公司</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,10 +444,10 @@
         <v>1702</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -458,10 +458,10 @@
         <v>1701</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -472,10 +472,10 @@
         <v>1601</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -486,10 +486,10 @@
         <v>1602</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -500,10 +500,10 @@
         <v>1501</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -514,10 +514,10 @@
         <v>2501</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ide updated by the way
</commit_message>
<xml_diff>
--- a/datasource/src/main/resources/arrangement.xlsx
+++ b/datasource/src/main/resources/arrangement.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data_content" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>floor</t>
   </si>
@@ -42,29 +42,153 @@
     <t>中国华电集团公司</t>
   </si>
   <si>
-    <t>上海华滨投资有限公司</t>
-  </si>
-  <si>
-    <t>华鑫国际信托有限公司</t>
-  </si>
-  <si>
     <t>华远星海运有限公司</t>
   </si>
   <si>
-    <t>华电重工股份有限公司上海分公司</t>
-  </si>
-  <si>
     <t>上海公司</t>
   </si>
   <si>
     <t>上海通华燃气轮机服务有限公司</t>
+  </si>
+  <si>
+    <t>english_name</t>
+  </si>
+  <si>
+    <t>CHINA HUADIAN CORPORATION SHANGHAI COMPANY</t>
+  </si>
+  <si>
+    <t>克拉克森航运经纪（上海）有限公司</t>
+  </si>
+  <si>
+    <t>上海烛龙影视文化有限公司</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SHANGHAI ZULON ENTERTAINMENT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>中国工商银行股份有限公司上海市世博支行</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>whole</t>
+  </si>
+  <si>
+    <t>1902.1903.1904</t>
+  </si>
+  <si>
+    <t>永和流体智控股份有限公司</t>
+  </si>
+  <si>
+    <t>上海信麟资产管理有限公司</t>
+  </si>
+  <si>
+    <t>上海普超企业管理咨询有限公司</t>
+  </si>
+  <si>
+    <t>上海金时股权投资基金管理有限公司</t>
+  </si>
+  <si>
+    <t>华保商业保理（上海）有限公司</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">浙江凤栖投资管理有限公司                      </t>
+  </si>
+  <si>
+    <t>上海申远建筑设计有限公司</t>
+  </si>
+  <si>
+    <t>奥可纳软件技术（上海）有限公司</t>
+  </si>
+  <si>
+    <t>华勤基信律师事务所</t>
+  </si>
+  <si>
+    <t>1602.1603.1604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">香港克拉克森柏拉图（亚洲）有限公司上海代表处
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLARKSONS PLATOU ASIA LIMITED SHANGHAI REPRESENTATIVE OFFICE </t>
+  </si>
+  <si>
+    <t>CLARKSONS PLATOU SHIPBROKING(SHANGHAI)CO.,LIMITED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SHANGHAI TONHUA GAS TURBING SERVICES CO.,LTD.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">同策资本  </t>
+  </si>
+  <si>
+    <t>TONG CAPITAL</t>
+  </si>
+  <si>
+    <r>
+      <t>上海华滨投资有限公司</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <charset val="134"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>SHANGHAI HUABIN INVESTMENT CO.,LTD</t>
+  </si>
+  <si>
+    <t>HUANYUAN STAR SHIPPING CO.,LTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">华鑫国际信托有限公司 </t>
+  </si>
+  <si>
+    <t>CHINA FORTUNE INTERNATIONAL TRUST CO. , LTD.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">华电重工股份有限公司上海分公司 </t>
+  </si>
+  <si>
+    <t>HUADIAN HEAVY INDUSTIES CO.,LTD SHANGHAI BRANCH</t>
+  </si>
+  <si>
+    <t>上海炫踪网络股份有限公司</t>
+  </si>
+  <si>
+    <t>SHINEZONE NETWORK CO.,LTD.</t>
+  </si>
+  <si>
+    <t>中国工商银行股份有限公司上海市世博支行</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +212,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <charset val="134"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <charset val="134"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri Light"/>
+      <charset val="134"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -106,7 +268,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -116,22 +278,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -407,118 +592,380 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="2" width="12.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="19.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="40.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="46" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2203</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2204</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2201</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1901</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1801</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1803</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>17</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1703.1704</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
         <v>1702</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="C13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
         <v>17</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B14" s="6">
         <v>1701</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>16</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
         <v>16</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B16" s="6">
         <v>1601</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1602</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="C16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>8</v>
+      </c>
+      <c r="B18" s="6">
+        <v>804</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>8</v>
+      </c>
+      <c r="B19" s="6">
+        <v>801</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1501</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>25</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2501</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="B20" s="6">
+        <v>703.70399999999995</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>7</v>
+      </c>
+      <c r="B21" s="6">
+        <v>701.702</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>5</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>3</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>2</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>1</v>
+      </c>
+      <c r="B25" s="6">
+        <v>101</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>